<commit_message>
Auto commit at 2025-11-02 10:12:50.35
</commit_message>
<xml_diff>
--- a/comprehensivedata/202510-202510.xlsx
+++ b/comprehensivedata/202510-202510.xlsx
@@ -330,12 +330,84 @@
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -343,78 +415,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -725,423 +725,413 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9" style="2"/>
-    <col min="6" max="6" width="7.125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9" style="2"/>
-    <col min="9" max="9" width="11.375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.75" style="2" customWidth="1"/>
-    <col min="12" max="13" width="10" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9" style="2"/>
-    <col min="15" max="15" width="10" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11.625" style="2" customWidth="1"/>
-    <col min="17" max="18" width="12.125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="14.875" style="2" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="16" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="7.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="1"/>
+    <col min="9" max="9" width="11.375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.75" style="1" customWidth="1"/>
+    <col min="12" max="13" width="10" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="1"/>
+    <col min="15" max="15" width="10" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.625" style="1" customWidth="1"/>
+    <col min="17" max="18" width="12.125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14.875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
     </row>
     <row r="2" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="4" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
     </row>
     <row r="3" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5" t="s">
+      <c r="K3" s="29"/>
+      <c r="L3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5" t="s">
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="8" t="s">
+      <c r="Q3" s="29"/>
+      <c r="R3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="S3" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="7" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="9"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="23"/>
     </row>
     <row r="5" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="2">
         <v>691.61</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="2">
         <v>412.83</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="24">
         <v>-322.35000000000002</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="24">
         <v>3430</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="24">
         <v>-90</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="2">
         <v>915</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7">
+      <c r="H5" s="2"/>
+      <c r="I5" s="2">
         <v>2567.4</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="13">
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="5">
         <v>4140</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="5">
         <v>3380</v>
       </c>
-      <c r="R5" s="13"/>
-      <c r="S5" s="14">
+      <c r="R5" s="5"/>
+      <c r="S5" s="6">
         <f>B5+C5+I5+P5+Q5+R5+G5</f>
         <v>12106.84</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="2">
         <v>214.54</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="2">
         <v>453.66</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="13">
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="5">
         <v>4015</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="5">
         <v>4800</v>
       </c>
-      <c r="R6" s="13"/>
-      <c r="S6" s="14">
+      <c r="R6" s="5"/>
+      <c r="S6" s="6">
         <f>B6+C6+D5+E5+F5+P6+Q6+R6</f>
         <v>12500.85</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="2">
         <v>136.97999999999999</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="2">
         <v>443.7</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="13">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="5">
         <v>2565</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q7" s="5">
         <v>2480</v>
       </c>
-      <c r="R7" s="13"/>
-      <c r="S7" s="14">
+      <c r="R7" s="5"/>
+      <c r="S7" s="6">
         <f>B7+C7+Q7+P7+R7</f>
         <v>5625.68</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="15">
         <f>B5+C5+B6+C6+B7+C7+D5+E5+F5</f>
         <v>5370.97</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="16">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="7">
         <f>G5</f>
         <v>915</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="8">
         <v>0</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="7">
         <f>I5</f>
         <v>2567.4</v>
       </c>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="21">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="9">
         <f>P5+P6+P7</f>
         <v>10720</v>
       </c>
-      <c r="Q8" s="20">
+      <c r="Q8" s="8">
         <f>Q5+Q6+Q7</f>
         <v>10660</v>
       </c>
-      <c r="R8" s="20">
+      <c r="R8" s="8">
         <f>R5+R6+R7</f>
         <v>0</v>
       </c>
-      <c r="S8" s="21">
+      <c r="S8" s="9">
         <f>Q8+P8+I8+B8+R8+G8</f>
         <v>30233.370000000003</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="16">
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="7">
         <v>1244.2</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="7">
         <v>528.55999999999995</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="7">
         <v>590</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="7">
         <v>7244</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="7">
         <v>7163</v>
       </c>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16">
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7">
         <f>L10+J10+I9</f>
         <v>9566.26</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="18">
         <f>B8</f>
         <v>5370.97</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="24">
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="12">
         <f>G8+G9</f>
         <v>915</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="13">
         <v>0</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="12">
         <f>I9+I8</f>
         <v>3811.6000000000004</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="18">
         <f>J9+K9</f>
         <v>1118.56</v>
       </c>
-      <c r="K10" s="27"/>
-      <c r="L10" s="25">
+      <c r="K10" s="20"/>
+      <c r="L10" s="18">
         <v>7203.5</v>
       </c>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="25">
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="18">
         <f>P8+Q8</f>
         <v>21380</v>
       </c>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="29">
+      <c r="Q10" s="20"/>
+      <c r="R10" s="14">
         <f>R9+R8</f>
         <v>0</v>
       </c>
-      <c r="S10" s="24">
+      <c r="S10" s="12">
         <f>SUM(B10:R10)</f>
         <v>39799.629999999997</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:O2"/>
@@ -1153,6 +1143,16 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:O3"/>
     <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="P10:Q10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto commit at 2025-11-03  9:02:31.72
</commit_message>
<xml_diff>
--- a/comprehensivedata/202510-202510.xlsx
+++ b/comprehensivedata/202510-202510.xlsx
@@ -381,40 +381,40 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -725,7 +725,7 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -751,96 +751,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
     </row>
     <row r="2" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="28" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
     </row>
     <row r="3" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="24" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29" t="s">
+      <c r="K3" s="21"/>
+      <c r="L3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29" t="s">
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="21" t="s">
+      <c r="Q3" s="21"/>
+      <c r="R3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="23" t="s">
+      <c r="S3" s="25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="29"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -856,8 +856,8 @@
       <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="2" t="s">
         <v>18</v>
       </c>
@@ -885,8 +885,8 @@
       <c r="Q4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="22"/>
-      <c r="S4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="25"/>
     </row>
     <row r="5" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
@@ -898,13 +898,13 @@
       <c r="C5" s="2">
         <v>412.83</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="22">
         <v>-322.35000000000002</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="22">
         <v>3430</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="22">
         <v>-90</v>
       </c>
       <c r="G5" s="2">
@@ -942,9 +942,9 @@
       <c r="C6" s="2">
         <v>453.66</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -976,9 +976,9 @@
       <c r="C7" s="2">
         <v>443.7</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1072,28 +1072,32 @@
       <c r="M9" s="7">
         <v>7163</v>
       </c>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+      <c r="N9" s="7">
+        <v>2853.82</v>
+      </c>
+      <c r="O9" s="7">
+        <v>970.6</v>
+      </c>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7">
         <f>L10+J10+I9</f>
-        <v>9566.26</v>
+        <v>11478.47</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="27">
         <f>B8</f>
         <v>5370.97</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="12">
         <f>G8+G9</f>
         <v>915</v>
@@ -1105,33 +1109,38 @@
         <f>I9+I8</f>
         <v>3811.6000000000004</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="27">
         <f>J9+K9</f>
         <v>1118.56</v>
       </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="18">
-        <v>7203.5</v>
-      </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="18">
+      <c r="K10" s="29"/>
+      <c r="L10" s="27">
+        <v>9115.7099999999991</v>
+      </c>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="27">
         <f>P8+Q8</f>
         <v>21380</v>
       </c>
-      <c r="Q10" s="20"/>
+      <c r="Q10" s="29"/>
       <c r="R10" s="14">
         <f>R9+R8</f>
         <v>0</v>
       </c>
       <c r="S10" s="12">
         <f>SUM(B10:R10)</f>
-        <v>39799.629999999997</v>
+        <v>41711.839999999997</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="P10:Q10"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:O2"/>
@@ -1148,11 +1157,6 @@
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="P10:Q10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>